<commit_message>
code now in classes and shit
</commit_message>
<xml_diff>
--- a/results/word2vec/word2vec_vectors.xlsx
+++ b/results/word2vec/word2vec_vectors.xlsx
@@ -20,52 +20,52 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="16">
   <si>
-    <t>cat</t>
+    <t>happy</t>
   </si>
   <si>
-    <t>dog</t>
+    <t>cute</t>
+  </si>
+  <si>
+    <t>big</t>
+  </si>
+  <si>
+    <t>bank</t>
   </si>
   <si>
     <t>money</t>
   </si>
   <si>
-    <t>big</t>
+    <t>small</t>
+  </si>
+  <si>
+    <t>deposit</t>
+  </si>
+  <si>
+    <t>&lt;EOL&gt;</t>
+  </si>
+  <si>
+    <t>fluffy</t>
+  </si>
+  <si>
+    <t>cat</t>
+  </si>
+  <si>
+    <t>withdraw</t>
+  </si>
+  <si>
+    <t>put</t>
   </si>
   <si>
     <t>&lt;SOL&gt;</t>
   </si>
   <si>
-    <t>&lt;EOL&gt;</t>
+    <t>good</t>
   </si>
   <si>
     <t>fun</t>
   </si>
   <si>
-    <t>bank</t>
-  </si>
-  <si>
-    <t>deposit</t>
-  </si>
-  <si>
-    <t>cute</t>
-  </si>
-  <si>
-    <t>fluffy</t>
-  </si>
-  <si>
-    <t>withdraw</t>
-  </si>
-  <si>
-    <t>good</t>
-  </si>
-  <si>
-    <t>put</t>
-  </si>
-  <si>
-    <t>happy</t>
-  </si>
-  <si>
-    <t>small</t>
+    <t>dog</t>
   </si>
 </sst>
 </file>
@@ -484,52 +484,52 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-0.1407701224088669</v>
+        <v>0.2970779240131378</v>
       </c>
       <c r="C2">
-        <v>-0.3438243567943573</v>
+        <v>0.2362677156925201</v>
       </c>
       <c r="D2">
-        <v>1.45950973033905</v>
+        <v>-1.0721195936203</v>
       </c>
       <c r="E2">
-        <v>0.9855896830558777</v>
+        <v>1.141375541687012</v>
       </c>
       <c r="F2">
-        <v>0.1216535195708275</v>
+        <v>-0.1212583854794502</v>
       </c>
       <c r="G2">
-        <v>0.9340542554855347</v>
+        <v>-0.8040529489517212</v>
       </c>
       <c r="H2">
-        <v>0.2978263795375824</v>
+        <v>0.1045998632907867</v>
       </c>
       <c r="I2">
-        <v>1.580844879150391</v>
+        <v>-0.2600601017475128</v>
       </c>
       <c r="J2">
-        <v>1.813691973686218</v>
+        <v>1.683956265449524</v>
       </c>
       <c r="K2">
-        <v>-0.1756659895181656</v>
+        <v>0.1801618635654449</v>
       </c>
       <c r="L2">
-        <v>-0.1941412836313248</v>
+        <v>-0.01065511908382177</v>
       </c>
       <c r="M2">
-        <v>1.815520286560059</v>
+        <v>-0.6924467086791992</v>
       </c>
       <c r="N2">
-        <v>0.5907908082008362</v>
+        <v>-0.2827032208442688</v>
       </c>
       <c r="O2">
-        <v>2.153151035308838</v>
+        <v>0.1846190989017487</v>
       </c>
       <c r="P2">
-        <v>0.1316060721874237</v>
+        <v>-1.535218834877014</v>
       </c>
       <c r="Q2">
-        <v>-0.09453552961349487</v>
+        <v>-0.2475148290395737</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -537,52 +537,52 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1.053076267242432</v>
+        <v>2.354334115982056</v>
       </c>
       <c r="C3">
-        <v>1.388987183570862</v>
+        <v>2.264865875244141</v>
       </c>
       <c r="D3">
-        <v>-0.08667795360088348</v>
+        <v>0.7118062973022461</v>
       </c>
       <c r="E3">
-        <v>0.4252538084983826</v>
+        <v>-0.16817706823349</v>
       </c>
       <c r="F3">
-        <v>-0.09538446366786957</v>
+        <v>-0.1991944909095764</v>
       </c>
       <c r="G3">
-        <v>0.7108666300773621</v>
+        <v>1.804075598716736</v>
       </c>
       <c r="H3">
-        <v>1.63006055355072</v>
+        <v>-0.3961351811885834</v>
       </c>
       <c r="I3">
-        <v>-0.2943755686283112</v>
+        <v>0.1747914254665375</v>
       </c>
       <c r="J3">
-        <v>-0.2204370200634003</v>
+        <v>1.996178865432739</v>
       </c>
       <c r="K3">
-        <v>1.921648383140564</v>
+        <v>1.273785829544067</v>
       </c>
       <c r="L3">
-        <v>1.533662080764771</v>
+        <v>-0.5432570576667786</v>
       </c>
       <c r="M3">
-        <v>-0.1790468394756317</v>
+        <v>0.2653968334197998</v>
       </c>
       <c r="N3">
-        <v>0.4039469957351685</v>
+        <v>0.03612400591373444</v>
       </c>
       <c r="O3">
-        <v>-0.1140376105904579</v>
+        <v>0.4028990268707275</v>
       </c>
       <c r="P3">
-        <v>1.731009364128113</v>
+        <v>2.391826868057251</v>
       </c>
       <c r="Q3">
-        <v>1.571873068809509</v>
+        <v>1.252487659454346</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -590,52 +590,52 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.7471188306808472</v>
+        <v>-0.04151675850152969</v>
       </c>
       <c r="C4">
-        <v>0.6735706329345703</v>
+        <v>-0.4170035123825073</v>
       </c>
       <c r="D4">
-        <v>0.7905300855636597</v>
+        <v>0.8399479389190674</v>
       </c>
       <c r="E4">
-        <v>0.5851918458938599</v>
+        <v>2.259941101074219</v>
       </c>
       <c r="F4">
-        <v>0.6693782210350037</v>
+        <v>1.586690664291382</v>
       </c>
       <c r="G4">
-        <v>-1.32434606552124</v>
+        <v>-0.1553910225629807</v>
       </c>
       <c r="H4">
-        <v>0.8347272276878357</v>
+        <v>4.216770648956299</v>
       </c>
       <c r="I4">
-        <v>0.8906739354133606</v>
+        <v>0.422846257686615</v>
       </c>
       <c r="J4">
-        <v>0.8349517583847046</v>
+        <v>-0.07238968461751938</v>
       </c>
       <c r="K4">
-        <v>0.6874213814735413</v>
+        <v>-0.001619363203644753</v>
       </c>
       <c r="L4">
-        <v>0.724681556224823</v>
+        <v>4.359067916870117</v>
       </c>
       <c r="M4">
-        <v>0.7942247986793518</v>
+        <v>2.423428773880005</v>
       </c>
       <c r="N4">
-        <v>0.4916408061981201</v>
+        <v>0.3741700947284698</v>
       </c>
       <c r="O4">
-        <v>0.986847460269928</v>
+        <v>0.544836163520813</v>
       </c>
       <c r="P4">
-        <v>0.6274304986000061</v>
+        <v>0.6296995282173157</v>
       </c>
       <c r="Q4">
-        <v>0.3994388580322266</v>
+        <v>-0.2149091511964798</v>
       </c>
     </row>
   </sheetData>
@@ -706,52 +706,52 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-0.5246996283531189</v>
+        <v>0.2799419462680817</v>
       </c>
       <c r="C2">
-        <v>0.4258191585540771</v>
+        <v>0.3875007927417755</v>
       </c>
       <c r="D2">
-        <v>1.77085816860199</v>
+        <v>1.30133330821991</v>
       </c>
       <c r="E2">
-        <v>0.5325497388839722</v>
+        <v>-1.18506932258606</v>
       </c>
       <c r="F2">
-        <v>1.868431568145752</v>
+        <v>0.1818582266569138</v>
       </c>
       <c r="G2">
-        <v>0.8537903428077698</v>
+        <v>1.12626576423645</v>
       </c>
       <c r="H2">
-        <v>-0.4108829498291016</v>
+        <v>0.818678617477417</v>
       </c>
       <c r="I2">
-        <v>1.655791640281677</v>
+        <v>0.3329710364341736</v>
       </c>
       <c r="J2">
-        <v>0.7018746137619019</v>
+        <v>-0.9079844951629639</v>
       </c>
       <c r="K2">
-        <v>-0.689211905002594</v>
+        <v>0.5580576062202454</v>
       </c>
       <c r="L2">
-        <v>-0.1596989780664444</v>
+        <v>0.9799321293830872</v>
       </c>
       <c r="M2">
-        <v>0.7020388841629028</v>
+        <v>0.8336647152900696</v>
       </c>
       <c r="N2">
-        <v>0.8926199078559875</v>
+        <v>0.5137634873390198</v>
       </c>
       <c r="O2">
-        <v>1.009743571281433</v>
+        <v>-0.1504926979541779</v>
       </c>
       <c r="P2">
-        <v>-1.223690867424011</v>
+        <v>0.8032546639442444</v>
       </c>
       <c r="Q2">
-        <v>-0.6965606808662415</v>
+        <v>0.2316898107528687</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -759,52 +759,52 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.7932643294334412</v>
+        <v>0.03829450532793999</v>
       </c>
       <c r="C3">
-        <v>1.859579563140869</v>
+        <v>0.8313469886779785</v>
       </c>
       <c r="D3">
-        <v>-0.6164346933364868</v>
+        <v>-0.005201621912419796</v>
       </c>
       <c r="E3">
-        <v>0.1398325711488724</v>
+        <v>-0.9794648885726929</v>
       </c>
       <c r="F3">
-        <v>1.806060671806335</v>
+        <v>-0.07949809730052948</v>
       </c>
       <c r="G3">
-        <v>0.879137396812439</v>
+        <v>0.7363561391830444</v>
       </c>
       <c r="H3">
-        <v>0.7633951306343079</v>
+        <v>-4.111281394958496</v>
       </c>
       <c r="I3">
-        <v>-0.1034808084368706</v>
+        <v>1.483073949813843</v>
       </c>
       <c r="J3">
-        <v>-1.14467978477478</v>
+        <v>0.9304032325744629</v>
       </c>
       <c r="K3">
-        <v>1.1528160572052</v>
+        <v>0.5153917074203491</v>
       </c>
       <c r="L3">
-        <v>1.358137011528015</v>
+        <v>-4.424899101257324</v>
       </c>
       <c r="M3">
-        <v>-1.234736680984497</v>
+        <v>-1.243481159210205</v>
       </c>
       <c r="N3">
-        <v>0.8425506949424744</v>
+        <v>1.366046547889709</v>
       </c>
       <c r="O3">
-        <v>-1.012205958366394</v>
+        <v>0.8531625866889954</v>
       </c>
       <c r="P3">
-        <v>0.5491549372673035</v>
+        <v>0.3669201135635376</v>
       </c>
       <c r="Q3">
-        <v>1.014956831932068</v>
+        <v>1.610428214073181</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -812,52 +812,52 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.09445135295391083</v>
+        <v>-2.277669429779053</v>
       </c>
       <c r="C4">
-        <v>0.6202230453491211</v>
+        <v>-1.438591837882996</v>
       </c>
       <c r="D4">
-        <v>0.290867805480957</v>
+        <v>0.4119365811347961</v>
       </c>
       <c r="E4">
-        <v>0.5015808343887329</v>
+        <v>1.237433433532715</v>
       </c>
       <c r="F4">
-        <v>0.8818609714508057</v>
+        <v>1.488447070121765</v>
       </c>
       <c r="G4">
-        <v>2.844364643096924</v>
+        <v>-0.8724464774131775</v>
       </c>
       <c r="H4">
-        <v>0.1860366761684418</v>
+        <v>0.7481347322463989</v>
       </c>
       <c r="I4">
-        <v>0.4264684319496155</v>
+        <v>1.362141966819763</v>
       </c>
       <c r="J4">
-        <v>0.1064200475811958</v>
+        <v>-1.142707347869873</v>
       </c>
       <c r="K4">
-        <v>0.3390945494174957</v>
+        <v>-1.14420747756958</v>
       </c>
       <c r="L4">
-        <v>0.3739628493785858</v>
+        <v>0.5489541888237</v>
       </c>
       <c r="M4">
-        <v>0.09274623543024063</v>
+        <v>0.7878854274749756</v>
       </c>
       <c r="N4">
-        <v>0.7695960998535156</v>
+        <v>1.612818717956543</v>
       </c>
       <c r="O4">
-        <v>0.1615851372480392</v>
+        <v>0.9420996904373169</v>
       </c>
       <c r="P4">
-        <v>0.01110491342842579</v>
+        <v>-0.4741256833076477</v>
       </c>
       <c r="Q4">
-        <v>0.4981310367584229</v>
+        <v>0.3105331063270569</v>
       </c>
     </row>
   </sheetData>
@@ -928,52 +928,52 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-0.3327348828315735</v>
+        <v>0.2885099351406097</v>
       </c>
       <c r="C2">
-        <v>0.04099740087985992</v>
+        <v>0.3118842542171478</v>
       </c>
       <c r="D2">
-        <v>1.61518394947052</v>
+        <v>0.1146068572998047</v>
       </c>
       <c r="E2">
-        <v>0.7590696811676025</v>
+        <v>-0.02184689044952393</v>
       </c>
       <c r="F2">
-        <v>0.9950425624847412</v>
+        <v>0.03029992058873177</v>
       </c>
       <c r="G2">
-        <v>0.8939223289489746</v>
+        <v>0.1611064076423645</v>
       </c>
       <c r="H2">
-        <v>-0.05652828514575958</v>
+        <v>0.4616392254829407</v>
       </c>
       <c r="I2">
-        <v>1.618318319320679</v>
+        <v>0.03645546734333038</v>
       </c>
       <c r="J2">
-        <v>1.25778329372406</v>
+        <v>0.38798588514328</v>
       </c>
       <c r="K2">
-        <v>-0.4324389398097992</v>
+        <v>0.3691097497940063</v>
       </c>
       <c r="L2">
-        <v>-0.1769201308488846</v>
+        <v>0.484638512134552</v>
       </c>
       <c r="M2">
-        <v>1.258779525756836</v>
+        <v>0.07060900330543518</v>
       </c>
       <c r="N2">
-        <v>0.7417053580284119</v>
+        <v>0.1155301332473755</v>
       </c>
       <c r="O2">
-        <v>1.58144736289978</v>
+        <v>0.0170632004737854</v>
       </c>
       <c r="P2">
-        <v>-0.5460423827171326</v>
+        <v>-0.3659820854663849</v>
       </c>
       <c r="Q2">
-        <v>-0.3955481052398682</v>
+        <v>-0.007912509143352509</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -981,52 +981,52 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.9231703281402588</v>
+        <v>1.196314334869385</v>
       </c>
       <c r="C3">
-        <v>1.624283313751221</v>
+        <v>1.54810643196106</v>
       </c>
       <c r="D3">
-        <v>-0.3515563309192657</v>
+        <v>0.3533023297786713</v>
       </c>
       <c r="E3">
-        <v>0.2825431823730469</v>
+        <v>-0.573820948600769</v>
       </c>
       <c r="F3">
-        <v>0.8553380966186523</v>
+        <v>-0.1393463015556335</v>
       </c>
       <c r="G3">
-        <v>0.7950019836425781</v>
+        <v>1.27021586894989</v>
       </c>
       <c r="H3">
-        <v>1.196727871894836</v>
+        <v>-2.253708362579346</v>
       </c>
       <c r="I3">
-        <v>-0.1989281922578812</v>
+        <v>0.8289327025413513</v>
       </c>
       <c r="J3">
-        <v>-0.6825584173202515</v>
+        <v>1.463291049003601</v>
       </c>
       <c r="K3">
-        <v>1.537232160568237</v>
+        <v>0.8945887684822083</v>
       </c>
       <c r="L3">
-        <v>1.445899486541748</v>
+        <v>-2.484078168869019</v>
       </c>
       <c r="M3">
-        <v>-0.7068917751312256</v>
+        <v>-0.4890421628952026</v>
       </c>
       <c r="N3">
-        <v>0.623248815536499</v>
+        <v>0.7010852694511414</v>
       </c>
       <c r="O3">
-        <v>-0.5631217956542969</v>
+        <v>0.6280307769775391</v>
       </c>
       <c r="P3">
-        <v>1.140082120895386</v>
+        <v>1.379373550415039</v>
       </c>
       <c r="Q3">
-        <v>1.293414950370789</v>
+        <v>1.431457996368408</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1034,52 +1034,52 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.4207850992679596</v>
+        <v>-1.159593105316162</v>
       </c>
       <c r="C4">
-        <v>0.6468968391418457</v>
+        <v>-0.9277976751327515</v>
       </c>
       <c r="D4">
-        <v>0.5406989455223083</v>
+        <v>0.6259422302246094</v>
       </c>
       <c r="E4">
-        <v>0.5433863401412964</v>
+        <v>1.748687267303467</v>
       </c>
       <c r="F4">
-        <v>0.7756196260452271</v>
+        <v>1.537568807601929</v>
       </c>
       <c r="G4">
-        <v>0.7600092887878418</v>
+        <v>-0.5139187574386597</v>
       </c>
       <c r="H4">
-        <v>0.5103819370269775</v>
+        <v>2.482452630996704</v>
       </c>
       <c r="I4">
-        <v>0.658571183681488</v>
+        <v>0.8924940824508667</v>
       </c>
       <c r="J4">
-        <v>0.4706858992576599</v>
+        <v>-0.6075485348701477</v>
       </c>
       <c r="K4">
-        <v>0.5132579803466797</v>
+        <v>-0.5729134082794189</v>
       </c>
       <c r="L4">
-        <v>0.5493221879005432</v>
+        <v>2.454010963439941</v>
       </c>
       <c r="M4">
-        <v>0.4434855282306671</v>
+        <v>1.60565710067749</v>
       </c>
       <c r="N4">
-        <v>0.6306184530258179</v>
+        <v>0.9934943914413452</v>
       </c>
       <c r="O4">
-        <v>0.5742163062095642</v>
+        <v>0.7434679269790649</v>
       </c>
       <c r="P4">
-        <v>0.3192677199840546</v>
+        <v>0.07778692245483398</v>
       </c>
       <c r="Q4">
-        <v>0.4487849473953247</v>
+        <v>0.04781197756528854</v>
       </c>
     </row>
   </sheetData>
@@ -1153,49 +1153,49 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.05799999833106995</v>
+        <v>0.0260000005364418</v>
       </c>
       <c r="D2">
-        <v>1.342000007629395</v>
+        <v>1.218999981880188</v>
       </c>
       <c r="E2">
-        <v>0.7720000147819519</v>
+        <v>1.873999953269958</v>
       </c>
       <c r="F2">
-        <v>0.5180000066757202</v>
+        <v>1.743000030517578</v>
       </c>
       <c r="G2">
-        <v>0.5</v>
+        <v>0.07299999892711639</v>
       </c>
       <c r="H2">
-        <v>0.03700000047683716</v>
+        <v>1.950999975204468</v>
       </c>
       <c r="I2">
-        <v>1.236999988555908</v>
+        <v>1.016000032424927</v>
       </c>
       <c r="J2">
-        <v>1.529000043869019</v>
+        <v>0.0689999982714653</v>
       </c>
       <c r="K2">
-        <v>0.007000000216066837</v>
+        <v>0.03200000151991844</v>
       </c>
       <c r="L2">
-        <v>0.02300000004470348</v>
+        <v>1.952000021934509</v>
       </c>
       <c r="M2">
-        <v>1.549000024795532</v>
+        <v>1.853999972343445</v>
       </c>
       <c r="N2">
-        <v>0.5189999938011169</v>
+        <v>1.136000037193298</v>
       </c>
       <c r="O2">
-        <v>1.424999952316284</v>
+        <v>1.064000010490417</v>
       </c>
       <c r="P2">
-        <v>0.01700000092387199</v>
+        <v>0.3980000019073486</v>
       </c>
       <c r="Q2">
-        <v>0.004999999888241291</v>
+        <v>0.3170000016689301</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1203,52 +1203,52 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.05799999833106995</v>
+        <v>0.0260000005364418</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1.050999999046326</v>
+        <v>0.9990000128746033</v>
       </c>
       <c r="E3">
-        <v>0.5070000290870667</v>
+        <v>1.746999979019165</v>
       </c>
       <c r="F3">
-        <v>0.2750000059604645</v>
+        <v>1.577000021934509</v>
       </c>
       <c r="G3">
-        <v>0.2660000026226044</v>
+        <v>0.0130000002682209</v>
       </c>
       <c r="H3">
-        <v>0.003000000026077032</v>
+        <v>1.91100001335144</v>
       </c>
       <c r="I3">
-        <v>0.9449999928474426</v>
+        <v>0.7910000085830688</v>
       </c>
       <c r="J3">
-        <v>1.28600001335144</v>
+        <v>0.0130000002682209</v>
       </c>
       <c r="K3">
-        <v>0.04199999943375587</v>
+        <v>0.01400000043213367</v>
       </c>
       <c r="L3">
-        <v>0.009999999776482582</v>
+        <v>1.924999952316284</v>
       </c>
       <c r="M3">
-        <v>1.307000041007996</v>
+        <v>1.723000049591064</v>
       </c>
       <c r="N3">
-        <v>0.2820000052452087</v>
+        <v>0.9110000133514404</v>
       </c>
       <c r="O3">
-        <v>1.154000043869019</v>
+        <v>0.8389999866485596</v>
       </c>
       <c r="P3">
-        <v>0.1070000007748604</v>
+        <v>0.2549999952316284</v>
       </c>
       <c r="Q3">
-        <v>0.04699999839067459</v>
+        <v>0.1729999929666519</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1256,52 +1256,52 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1.342000007629395</v>
+        <v>1.218999981880188</v>
       </c>
       <c r="C4">
-        <v>1.050999999046326</v>
+        <v>0.9990000128746033</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.1630000025033951</v>
+        <v>0.335999995470047</v>
       </c>
       <c r="F4">
-        <v>0.3490000069141388</v>
+        <v>0.1840000003576279</v>
       </c>
       <c r="G4">
-        <v>0.3610000014305115</v>
+        <v>0.8550000190734863</v>
       </c>
       <c r="H4">
-        <v>1.103999972343445</v>
+        <v>0.6710000038146973</v>
       </c>
       <c r="I4">
-        <v>0.006000000052154064</v>
+        <v>0.03500000014901161</v>
       </c>
       <c r="J4">
-        <v>0.03599999845027924</v>
+        <v>0.8470000028610229</v>
       </c>
       <c r="K4">
-        <v>1.330000042915344</v>
+        <v>1</v>
       </c>
       <c r="L4">
-        <v>1.184000015258789</v>
+        <v>0.7220000028610229</v>
       </c>
       <c r="M4">
-        <v>0.03999999910593033</v>
+        <v>0.3129999935626984</v>
       </c>
       <c r="N4">
-        <v>0.3429999947547913</v>
+        <v>0.007000000216066837</v>
       </c>
       <c r="O4">
-        <v>0.007000000216066837</v>
+        <v>0.02700000070035458</v>
       </c>
       <c r="P4">
-        <v>1.490000009536743</v>
+        <v>0.5249999761581421</v>
       </c>
       <c r="Q4">
-        <v>1.343000054359436</v>
+        <v>0.4869999885559082</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -1309,52 +1309,52 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.7720000147819519</v>
+        <v>1.873999953269958</v>
       </c>
       <c r="C5">
-        <v>0.5070000290870667</v>
+        <v>1.746999979019165</v>
       </c>
       <c r="D5">
-        <v>0.1630000025033951</v>
+        <v>0.335999995470047</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.04600000008940697</v>
+        <v>0.0260000005364418</v>
       </c>
       <c r="G5">
-        <v>0.04800000041723251</v>
+        <v>1.641999959945679</v>
       </c>
       <c r="H5">
-        <v>0.5490000247955322</v>
+        <v>0.09700000286102295</v>
       </c>
       <c r="I5">
-        <v>0.1080000028014183</v>
+        <v>0.5170000195503235</v>
       </c>
       <c r="J5">
-        <v>0.3070000112056732</v>
+        <v>1.636000037193298</v>
       </c>
       <c r="K5">
-        <v>0.7649999856948853</v>
+        <v>1.735999941825867</v>
       </c>
       <c r="L5">
-        <v>0.6230000257492065</v>
+        <v>0.1209999993443489</v>
       </c>
       <c r="M5">
-        <v>0.3230000138282776</v>
+        <v>0.002000000094994903</v>
       </c>
       <c r="N5">
-        <v>0.04100000113248825</v>
+        <v>0.4070000052452087</v>
       </c>
       <c r="O5">
-        <v>0.2179999947547913</v>
+        <v>0.4760000109672546</v>
       </c>
       <c r="P5">
-        <v>0.9359999895095825</v>
+        <v>1.246000051498413</v>
       </c>
       <c r="Q5">
-        <v>0.7779999971389771</v>
+        <v>1.279999971389771</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1362,52 +1362,52 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.5180000066757202</v>
+        <v>1.743000030517578</v>
       </c>
       <c r="C6">
-        <v>0.2750000059604645</v>
+        <v>1.577000021934509</v>
       </c>
       <c r="D6">
-        <v>0.3490000069141388</v>
+        <v>0.1840000003576279</v>
       </c>
       <c r="E6">
-        <v>0.04600000008940697</v>
+        <v>0.0260000005364418</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0.001000000047497451</v>
+        <v>1.452000021934509</v>
       </c>
       <c r="H6">
-        <v>0.3129999935626984</v>
+        <v>0.2070000022649765</v>
       </c>
       <c r="I6">
-        <v>0.2720000147819519</v>
+        <v>0.3319999873638153</v>
       </c>
       <c r="J6">
-        <v>0.550000011920929</v>
+        <v>1.447000026702881</v>
       </c>
       <c r="K6">
-        <v>0.4979999959468842</v>
+        <v>1.572999954223633</v>
       </c>
       <c r="L6">
-        <v>0.3729999959468842</v>
+        <v>0.2409999966621399</v>
       </c>
       <c r="M6">
-        <v>0.5690000057220459</v>
+        <v>0.02099999971687794</v>
       </c>
       <c r="N6">
-        <v>0.001000000047497451</v>
+        <v>0.239999994635582</v>
       </c>
       <c r="O6">
-        <v>0.4320000112056732</v>
+        <v>0.296999990940094</v>
       </c>
       <c r="P6">
-        <v>0.6579999923706055</v>
+        <v>1.037999987602234</v>
       </c>
       <c r="Q6">
-        <v>0.5120000243186951</v>
+        <v>1.057000041007996</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1415,52 +1415,52 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.5</v>
+        <v>0.07299999892711639</v>
       </c>
       <c r="C7">
-        <v>0.2660000026226044</v>
+        <v>0.0130000002682209</v>
       </c>
       <c r="D7">
-        <v>0.3610000014305115</v>
+        <v>0.8550000190734863</v>
       </c>
       <c r="E7">
-        <v>0.04800000041723251</v>
+        <v>1.641999959945679</v>
       </c>
       <c r="F7">
-        <v>0.001000000047497451</v>
+        <v>1.452000021934509</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>0.3019999861717224</v>
+        <v>1.870000004768372</v>
       </c>
       <c r="I7">
-        <v>0.2820000052452087</v>
+        <v>0.6430000066757202</v>
       </c>
       <c r="J7">
-        <v>0.5600000023841858</v>
+        <v>0.00800000037997961</v>
       </c>
       <c r="K7">
-        <v>0.4839999973773956</v>
+        <v>0.03999999910593033</v>
       </c>
       <c r="L7">
-        <v>0.3619999885559082</v>
+        <v>1.891999959945679</v>
       </c>
       <c r="M7">
-        <v>0.5789999961853027</v>
+        <v>1.61899995803833</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>0.7630000114440918</v>
       </c>
       <c r="O7">
-        <v>0.4420000016689301</v>
+        <v>0.6880000233650208</v>
       </c>
       <c r="P7">
-        <v>0.6420000195503235</v>
+        <v>0.1620000004768372</v>
       </c>
       <c r="Q7">
-        <v>0.4970000088214874</v>
+        <v>0.09300000220537186</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1468,52 +1468,52 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.03700000047683716</v>
+        <v>1.950999975204468</v>
       </c>
       <c r="C8">
-        <v>0.003000000026077032</v>
+        <v>1.91100001335144</v>
       </c>
       <c r="D8">
-        <v>1.103999972343445</v>
+        <v>0.6710000038146973</v>
       </c>
       <c r="E8">
-        <v>0.5490000247955322</v>
+        <v>0.09700000286102295</v>
       </c>
       <c r="F8">
-        <v>0.3129999935626984</v>
+        <v>0.2070000022649765</v>
       </c>
       <c r="G8">
-        <v>0.3019999861717224</v>
+        <v>1.870000004768372</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>0.996999979019165</v>
+        <v>0.9120000004768372</v>
       </c>
       <c r="J8">
-        <v>1.330000042915344</v>
+        <v>1.838000059127808</v>
       </c>
       <c r="K8">
-        <v>0.02700000070035458</v>
+        <v>1.858999967575073</v>
       </c>
       <c r="L8">
-        <v>0.003000000026077032</v>
+        <v>0.001000000047497451</v>
       </c>
       <c r="M8">
-        <v>1.35099995136261</v>
+        <v>0.0989999994635582</v>
       </c>
       <c r="N8">
-        <v>0.3190000057220459</v>
+        <v>0.7730000019073486</v>
       </c>
       <c r="O8">
-        <v>1.203999996185303</v>
+        <v>0.8669999837875366</v>
       </c>
       <c r="P8">
-        <v>0.0820000022649765</v>
+        <v>1.638000011444092</v>
       </c>
       <c r="Q8">
-        <v>0.02999999932944775</v>
+        <v>1.641999959945679</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1521,52 +1521,52 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1.236999988555908</v>
+        <v>1.016000032424927</v>
       </c>
       <c r="C9">
-        <v>0.9449999928474426</v>
+        <v>0.7910000085830688</v>
       </c>
       <c r="D9">
-        <v>0.006000000052154064</v>
+        <v>0.03500000014901161</v>
       </c>
       <c r="E9">
-        <v>0.1080000028014183</v>
+        <v>0.5170000195503235</v>
       </c>
       <c r="F9">
-        <v>0.2720000147819519</v>
+        <v>0.3319999873638153</v>
       </c>
       <c r="G9">
-        <v>0.2820000052452087</v>
+        <v>0.6430000066757202</v>
       </c>
       <c r="H9">
-        <v>0.996999979019165</v>
+        <v>0.9120000004768372</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>0.06300000101327896</v>
+        <v>0.6549999713897705</v>
       </c>
       <c r="K9">
-        <v>1.22599995136261</v>
+        <v>0.8220000267028809</v>
       </c>
       <c r="L9">
-        <v>1.077999949455261</v>
+        <v>0.9649999737739563</v>
       </c>
       <c r="M9">
-        <v>0.07000000029802322</v>
+        <v>0.4970000088214874</v>
       </c>
       <c r="N9">
-        <v>0.2660000026226044</v>
+        <v>0.01099999994039536</v>
       </c>
       <c r="O9">
-        <v>0.02300000004470348</v>
+        <v>0.001000000047497451</v>
       </c>
       <c r="P9">
-        <v>1.39300000667572</v>
+        <v>0.3109999895095825</v>
       </c>
       <c r="Q9">
-        <v>1.240000009536743</v>
+        <v>0.2960000038146973</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1574,52 +1574,52 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1.529000043869019</v>
+        <v>0.0689999982714653</v>
       </c>
       <c r="C10">
-        <v>1.28600001335144</v>
+        <v>0.0130000002682209</v>
       </c>
       <c r="D10">
-        <v>0.03599999845027924</v>
+        <v>0.8470000028610229</v>
       </c>
       <c r="E10">
-        <v>0.3070000112056732</v>
+        <v>1.636000037193298</v>
       </c>
       <c r="F10">
-        <v>0.550000011920929</v>
+        <v>1.447000026702881</v>
       </c>
       <c r="G10">
-        <v>0.5600000023841858</v>
+        <v>0.00800000037997961</v>
       </c>
       <c r="H10">
-        <v>1.330000042915344</v>
+        <v>1.838000059127808</v>
       </c>
       <c r="I10">
-        <v>0.06300000101327896</v>
+        <v>0.6549999713897705</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <v>1.534999966621399</v>
+        <v>0.01899999938905239</v>
       </c>
       <c r="L10">
-        <v>1.404999971389771</v>
+        <v>1.858999967575073</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>1.60699999332428</v>
       </c>
       <c r="N10">
-        <v>0.5379999876022339</v>
+        <v>0.765999972820282</v>
       </c>
       <c r="O10">
-        <v>0.01099999994039536</v>
+        <v>0.7020000219345093</v>
       </c>
       <c r="P10">
-        <v>1.669000029563904</v>
+        <v>0.2150000035762787</v>
       </c>
       <c r="Q10">
-        <v>1.544999957084656</v>
+        <v>0.1169999986886978</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1627,52 +1627,52 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.007000000216066837</v>
+        <v>0.03200000151991844</v>
       </c>
       <c r="C11">
-        <v>0.04199999943375587</v>
+        <v>0.01400000043213367</v>
       </c>
       <c r="D11">
-        <v>1.330000042915344</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>0.7649999856948853</v>
+        <v>1.735999941825867</v>
       </c>
       <c r="F11">
-        <v>0.4979999959468842</v>
+        <v>1.572999954223633</v>
       </c>
       <c r="G11">
-        <v>0.4839999973773956</v>
+        <v>0.03999999910593033</v>
       </c>
       <c r="H11">
-        <v>0.02700000070035458</v>
+        <v>1.858999967575073</v>
       </c>
       <c r="I11">
-        <v>1.22599995136261</v>
+        <v>0.8220000267028809</v>
       </c>
       <c r="J11">
-        <v>1.534999966621399</v>
+        <v>0.01899999938905239</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
-        <v>0.01200000010430813</v>
+        <v>1.870000004768372</v>
       </c>
       <c r="M11">
-        <v>1.554000020027161</v>
+        <v>1.705000042915344</v>
       </c>
       <c r="N11">
-        <v>0.5040000081062317</v>
+        <v>0.9269999861717224</v>
       </c>
       <c r="O11">
-        <v>1.422000050544739</v>
+        <v>0.8700000047683716</v>
       </c>
       <c r="P11">
-        <v>0.01600000075995922</v>
+        <v>0.3440000116825104</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>0.2240000069141388</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1680,52 +1680,52 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.02300000004470348</v>
+        <v>1.952000021934509</v>
       </c>
       <c r="C12">
-        <v>0.009999999776482582</v>
+        <v>1.924999952316284</v>
       </c>
       <c r="D12">
-        <v>1.184000015258789</v>
+        <v>0.7220000028610229</v>
       </c>
       <c r="E12">
-        <v>0.6230000257492065</v>
+        <v>0.1209999993443489</v>
       </c>
       <c r="F12">
-        <v>0.3729999959468842</v>
+        <v>0.2409999966621399</v>
       </c>
       <c r="G12">
-        <v>0.3619999885559082</v>
+        <v>1.891999959945679</v>
       </c>
       <c r="H12">
-        <v>0.003000000026077032</v>
+        <v>0.001000000047497451</v>
       </c>
       <c r="I12">
-        <v>1.077999949455261</v>
+        <v>0.9649999737739563</v>
       </c>
       <c r="J12">
-        <v>1.404999971389771</v>
+        <v>1.858999967575073</v>
       </c>
       <c r="K12">
-        <v>0.01200000010430813</v>
+        <v>1.870000004768372</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>1.425999999046326</v>
+        <v>0.1239999979734421</v>
       </c>
       <c r="N12">
-        <v>0.3799999952316284</v>
+        <v>0.824999988079071</v>
       </c>
       <c r="O12">
-        <v>1.281999945640564</v>
+        <v>0.9210000038146973</v>
       </c>
       <c r="P12">
-        <v>0.05400000140070915</v>
+        <v>1.677000045776367</v>
       </c>
       <c r="Q12">
-        <v>0.01400000043213367</v>
+        <v>1.682000041007996</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1733,52 +1733,52 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>1.549000024795532</v>
+        <v>1.853999972343445</v>
       </c>
       <c r="C13">
-        <v>1.307000041007996</v>
+        <v>1.723000049591064</v>
       </c>
       <c r="D13">
-        <v>0.03999999910593033</v>
+        <v>0.3129999935626984</v>
       </c>
       <c r="E13">
-        <v>0.3230000138282776</v>
+        <v>0.002000000094994903</v>
       </c>
       <c r="F13">
-        <v>0.5690000057220459</v>
+        <v>0.02099999971687794</v>
       </c>
       <c r="G13">
-        <v>0.5789999961853027</v>
+        <v>1.61899995803833</v>
       </c>
       <c r="H13">
-        <v>1.35099995136261</v>
+        <v>0.0989999994635582</v>
       </c>
       <c r="I13">
-        <v>0.07000000029802322</v>
+        <v>0.4970000088214874</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>1.60699999332428</v>
       </c>
       <c r="K13">
-        <v>1.554000020027161</v>
+        <v>1.705000042915344</v>
       </c>
       <c r="L13">
-        <v>1.425999999046326</v>
+        <v>0.1239999979734421</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
       <c r="N13">
-        <v>0.5569999814033508</v>
+        <v>0.386000007390976</v>
       </c>
       <c r="O13">
-        <v>0.0130000002682209</v>
+        <v>0.4569999873638153</v>
       </c>
       <c r="P13">
-        <v>1.685999989509583</v>
+        <v>1.240000009536743</v>
       </c>
       <c r="Q13">
-        <v>1.564000010490417</v>
+        <v>1.258999943733215</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1786,52 +1786,52 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.5189999938011169</v>
+        <v>1.136000037193298</v>
       </c>
       <c r="C14">
-        <v>0.2820000052452087</v>
+        <v>0.9110000133514404</v>
       </c>
       <c r="D14">
-        <v>0.3429999947547913</v>
+        <v>0.007000000216066837</v>
       </c>
       <c r="E14">
-        <v>0.04100000113248825</v>
+        <v>0.4070000052452087</v>
       </c>
       <c r="F14">
-        <v>0.001000000047497451</v>
+        <v>0.239999994635582</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>0.7630000114440918</v>
       </c>
       <c r="H14">
-        <v>0.3190000057220459</v>
+        <v>0.7730000019073486</v>
       </c>
       <c r="I14">
-        <v>0.2660000026226044</v>
+        <v>0.01099999994039536</v>
       </c>
       <c r="J14">
-        <v>0.5379999876022339</v>
+        <v>0.765999972820282</v>
       </c>
       <c r="K14">
-        <v>0.5040000081062317</v>
+        <v>0.9269999861717224</v>
       </c>
       <c r="L14">
-        <v>0.3799999952316284</v>
+        <v>0.824999988079071</v>
       </c>
       <c r="M14">
-        <v>0.5569999814033508</v>
+        <v>0.386000007390976</v>
       </c>
       <c r="N14">
         <v>0</v>
       </c>
       <c r="O14">
-        <v>0.4230000078678131</v>
+        <v>0.007000000216066837</v>
       </c>
       <c r="P14">
-        <v>0.6639999747276306</v>
+        <v>0.4259999990463257</v>
       </c>
       <c r="Q14">
-        <v>0.5170000195503235</v>
+        <v>0.4000000059604645</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1839,52 +1839,52 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>1.424999952316284</v>
+        <v>1.064000010490417</v>
       </c>
       <c r="C15">
-        <v>1.154000043869019</v>
+        <v>0.8389999866485596</v>
       </c>
       <c r="D15">
+        <v>0.02700000070035458</v>
+      </c>
+      <c r="E15">
+        <v>0.4760000109672546</v>
+      </c>
+      <c r="F15">
+        <v>0.296999990940094</v>
+      </c>
+      <c r="G15">
+        <v>0.6880000233650208</v>
+      </c>
+      <c r="H15">
+        <v>0.8669999837875366</v>
+      </c>
+      <c r="I15">
+        <v>0.001000000047497451</v>
+      </c>
+      <c r="J15">
+        <v>0.7020000219345093</v>
+      </c>
+      <c r="K15">
+        <v>0.8700000047683716</v>
+      </c>
+      <c r="L15">
+        <v>0.9210000038146973</v>
+      </c>
+      <c r="M15">
+        <v>0.4569999873638153</v>
+      </c>
+      <c r="N15">
         <v>0.007000000216066837</v>
       </c>
-      <c r="E15">
-        <v>0.2179999947547913</v>
-      </c>
-      <c r="F15">
-        <v>0.4320000112056732</v>
-      </c>
-      <c r="G15">
-        <v>0.4420000016689301</v>
-      </c>
-      <c r="H15">
-        <v>1.203999996185303</v>
-      </c>
-      <c r="I15">
-        <v>0.02300000004470348</v>
-      </c>
-      <c r="J15">
-        <v>0.01099999994039536</v>
-      </c>
-      <c r="K15">
-        <v>1.422000050544739</v>
-      </c>
-      <c r="L15">
-        <v>1.281999945640564</v>
-      </c>
-      <c r="M15">
-        <v>0.0130000002682209</v>
-      </c>
-      <c r="N15">
-        <v>0.4230000078678131</v>
-      </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15">
-        <v>1.572000026702881</v>
+        <v>0.3400000035762787</v>
       </c>
       <c r="Q15">
-        <v>1.434000015258789</v>
+        <v>0.3300000131130219</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1892,52 +1892,52 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.01700000092387199</v>
+        <v>0.3980000019073486</v>
       </c>
       <c r="C16">
-        <v>0.1070000007748604</v>
+        <v>0.2549999952316284</v>
       </c>
       <c r="D16">
-        <v>1.490000009536743</v>
+        <v>0.5249999761581421</v>
       </c>
       <c r="E16">
-        <v>0.9359999895095825</v>
+        <v>1.246000051498413</v>
       </c>
       <c r="F16">
-        <v>0.6579999923706055</v>
+        <v>1.037999987602234</v>
       </c>
       <c r="G16">
-        <v>0.6420000195503235</v>
+        <v>0.1620000004768372</v>
       </c>
       <c r="H16">
-        <v>0.0820000022649765</v>
+        <v>1.638000011444092</v>
       </c>
       <c r="I16">
-        <v>1.39300000667572</v>
+        <v>0.3109999895095825</v>
       </c>
       <c r="J16">
-        <v>1.669000029563904</v>
+        <v>0.2150000035762787</v>
       </c>
       <c r="K16">
-        <v>0.01600000075995922</v>
+        <v>0.3440000116825104</v>
       </c>
       <c r="L16">
-        <v>0.05400000140070915</v>
+        <v>1.677000045776367</v>
       </c>
       <c r="M16">
-        <v>1.685999989509583</v>
+        <v>1.240000009536743</v>
       </c>
       <c r="N16">
-        <v>0.6639999747276306</v>
+        <v>0.4259999990463257</v>
       </c>
       <c r="O16">
-        <v>1.572000026702881</v>
+        <v>0.3400000035762787</v>
       </c>
       <c r="P16">
         <v>0</v>
       </c>
       <c r="Q16">
-        <v>0.0130000002682209</v>
+        <v>0.03200000151991844</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1945,49 +1945,49 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.004999999888241291</v>
+        <v>0.3170000016689301</v>
       </c>
       <c r="C17">
-        <v>0.04699999839067459</v>
+        <v>0.1729999929666519</v>
       </c>
       <c r="D17">
-        <v>1.343000054359436</v>
+        <v>0.4869999885559082</v>
       </c>
       <c r="E17">
-        <v>0.7779999971389771</v>
+        <v>1.279999971389771</v>
       </c>
       <c r="F17">
-        <v>0.5120000243186951</v>
+        <v>1.057000041007996</v>
       </c>
       <c r="G17">
-        <v>0.4970000088214874</v>
+        <v>0.09300000220537186</v>
       </c>
       <c r="H17">
-        <v>0.02999999932944775</v>
+        <v>1.641999959945679</v>
       </c>
       <c r="I17">
-        <v>1.240000009536743</v>
+        <v>0.2960000038146973</v>
       </c>
       <c r="J17">
-        <v>1.544999957084656</v>
+        <v>0.1169999986886978</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>0.2240000069141388</v>
       </c>
       <c r="L17">
-        <v>0.01400000043213367</v>
+        <v>1.682000041007996</v>
       </c>
       <c r="M17">
-        <v>1.564000010490417</v>
+        <v>1.258999943733215</v>
       </c>
       <c r="N17">
-        <v>0.5170000195503235</v>
+        <v>0.4000000059604645</v>
       </c>
       <c r="O17">
-        <v>1.434000015258789</v>
+        <v>0.3300000131130219</v>
       </c>
       <c r="P17">
-        <v>0.0130000002682209</v>
+        <v>0.03200000151991844</v>
       </c>
       <c r="Q17">
         <v>0</v>
@@ -2064,49 +2064,49 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.8259999752044678</v>
+        <v>0.421999990940094</v>
       </c>
       <c r="D2">
-        <v>2.331000089645386</v>
+        <v>1.98199999332428</v>
       </c>
       <c r="E2">
-        <v>1.271999955177307</v>
+        <v>3.418999910354614</v>
       </c>
       <c r="F2">
-        <v>1.376000046730042</v>
+        <v>3.020999908447266</v>
       </c>
       <c r="G2">
-        <v>1.279000043869019</v>
+        <v>0.6620000004768372</v>
       </c>
       <c r="H2">
-        <v>0.3989999890327454</v>
+        <v>5.019999980926514</v>
       </c>
       <c r="I2">
-        <v>2.263000011444092</v>
+        <v>2.099999904632568</v>
       </c>
       <c r="J2">
-        <v>2.260999917984009</v>
+        <v>0.6209999918937683</v>
       </c>
       <c r="K2">
-        <v>0.6290000081062317</v>
+        <v>0.6650000214576721</v>
       </c>
       <c r="L2">
-        <v>0.5600000023841858</v>
+        <v>5.162000179290771</v>
       </c>
       <c r="M2">
-        <v>2.278000116348267</v>
+        <v>3.246000051498413</v>
       </c>
       <c r="N2">
-        <v>1.134999990463257</v>
+        <v>2.216000080108643</v>
       </c>
       <c r="O2">
-        <v>2.427999973297119</v>
+        <v>2.005000114440918</v>
       </c>
       <c r="P2">
-        <v>0.3210000097751617</v>
+        <v>1.411999940872192</v>
       </c>
       <c r="Q2">
-        <v>0.3770000040531158</v>
+        <v>1.264999985694885</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -2114,52 +2114,52 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.8259999752044678</v>
+        <v>0.421999990940094</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>2.528000116348267</v>
+        <v>1.970000028610229</v>
       </c>
       <c r="E3">
-        <v>1.524999976158142</v>
+        <v>3.431999921798706</v>
       </c>
       <c r="F3">
-        <v>1.23199999332428</v>
+        <v>3.000999927520752</v>
       </c>
       <c r="G3">
-        <v>1.195000052452087</v>
+        <v>0.5210000276565552</v>
       </c>
       <c r="H3">
-        <v>0.4589999914169312</v>
+        <v>5.109000205993652</v>
       </c>
       <c r="I3">
-        <v>2.41100001335144</v>
+        <v>1.97599995136261</v>
       </c>
       <c r="J3">
-        <v>2.614000082015991</v>
+        <v>0.3400000035762787</v>
       </c>
       <c r="K3">
-        <v>0.5</v>
+        <v>0.7459999918937683</v>
       </c>
       <c r="L3">
-        <v>0.2980000078678131</v>
+        <v>5.264999866485596</v>
       </c>
       <c r="M3">
-        <v>2.638000011444092</v>
+        <v>3.259999990463257</v>
       </c>
       <c r="N3">
-        <v>1.222000002861023</v>
+        <v>2.108999967575073</v>
       </c>
       <c r="O3">
-        <v>2.676000118255615</v>
+        <v>1.929999947547913</v>
       </c>
       <c r="P3">
-        <v>0.828000009059906</v>
+        <v>1.223999977111816</v>
       </c>
       <c r="Q3">
-        <v>0.5820000171661377</v>
+        <v>1.032999992370605</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -2167,52 +2167,52 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>2.331000089645386</v>
+        <v>1.98199999332428</v>
       </c>
       <c r="C4">
-        <v>2.528000116348267</v>
+        <v>1.970000028610229</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1.065000057220459</v>
+        <v>1.462000012397766</v>
       </c>
       <c r="F4">
-        <v>1.376999974250793</v>
+        <v>1.039999961853027</v>
       </c>
       <c r="G4">
-        <v>1.371999979019165</v>
+        <v>1.46399998664856</v>
       </c>
       <c r="H4">
-        <v>2.279000043869019</v>
+        <v>3.219000101089478</v>
       </c>
       <c r="I4">
-        <v>0.193000003695488</v>
+        <v>0.5509999990463257</v>
       </c>
       <c r="J4">
-        <v>0.492000013589859</v>
+        <v>1.682000041007996</v>
       </c>
       <c r="K4">
-        <v>2.78600001335144</v>
+        <v>1.340000033378601</v>
       </c>
       <c r="L4">
-        <v>2.538000106811523</v>
+        <v>3.395999908447266</v>
       </c>
       <c r="M4">
-        <v>0.5130000114440918</v>
+        <v>1.292999982833862</v>
       </c>
       <c r="N4">
-        <v>1.312000036239624</v>
+        <v>0.5059999823570251</v>
       </c>
       <c r="O4">
-        <v>0.2169999927282333</v>
+        <v>0.3140000104904175</v>
       </c>
       <c r="P4">
-        <v>2.634999990463257</v>
+        <v>1.258999943733215</v>
       </c>
       <c r="Q4">
-        <v>2.599999904632568</v>
+        <v>1.228999972343445</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -2220,52 +2220,52 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1.271999955177307</v>
+        <v>3.418999910354614</v>
       </c>
       <c r="C5">
-        <v>1.524999976158142</v>
+        <v>3.431999921798706</v>
       </c>
       <c r="D5">
-        <v>1.065000057220459</v>
+        <v>1.462000012397766</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.6620000004768372</v>
+        <v>0.4860000014305115</v>
       </c>
       <c r="G5">
-        <v>0.5720000267028809</v>
+        <v>2.924999952316284</v>
       </c>
       <c r="H5">
-        <v>1.22599995136261</v>
+        <v>1.896000027656555</v>
       </c>
       <c r="I5">
-        <v>0.9919999837875366</v>
+        <v>1.644000053405762</v>
       </c>
       <c r="J5">
-        <v>1.08899998664856</v>
+        <v>3.141999959945679</v>
       </c>
       <c r="K5">
-        <v>1.730999946594238</v>
+        <v>2.775000095367432</v>
       </c>
       <c r="L5">
-        <v>1.493000030517578</v>
+        <v>2.098000049591064</v>
       </c>
       <c r="M5">
-        <v>1.11300003528595</v>
+        <v>0.1899999976158142</v>
       </c>
       <c r="N5">
-        <v>0.3519999980926514</v>
+        <v>1.48800003528595</v>
       </c>
       <c r="O5">
-        <v>1.179999947547913</v>
+        <v>1.567000031471252</v>
       </c>
       <c r="P5">
-        <v>1.577999949455261</v>
+        <v>2.592999935150146</v>
       </c>
       <c r="Q5">
-        <v>1.537999987602234</v>
+        <v>2.630000114440918</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -2273,52 +2273,52 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1.376000046730042</v>
+        <v>3.020999908447266</v>
       </c>
       <c r="C6">
-        <v>1.23199999332428</v>
+        <v>3.000999927520752</v>
       </c>
       <c r="D6">
-        <v>1.376999974250793</v>
+        <v>1.039999961853027</v>
       </c>
       <c r="E6">
-        <v>0.6620000004768372</v>
+        <v>0.4860000014305115</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0.1190000027418137</v>
+        <v>2.493000030517578</v>
       </c>
       <c r="H6">
-        <v>1.13699996471405</v>
+        <v>2.355999946594238</v>
       </c>
       <c r="I6">
-        <v>1.230000019073486</v>
+        <v>1.162999987602234</v>
       </c>
       <c r="J6">
-        <v>1.590000033378601</v>
+        <v>2.700999975204468</v>
       </c>
       <c r="K6">
-        <v>1.603999972343445</v>
+        <v>2.374000072479248</v>
       </c>
       <c r="L6">
-        <v>1.332000017166138</v>
+        <v>2.558000087738037</v>
       </c>
       <c r="M6">
-        <v>1.61899995803833</v>
+        <v>0.3589999973773956</v>
       </c>
       <c r="N6">
-        <v>0.3729999959468842</v>
+        <v>1.004999995231628</v>
       </c>
       <c r="O6">
-        <v>1.547999978065491</v>
+        <v>1.103999972343445</v>
       </c>
       <c r="P6">
-        <v>1.631999969482422</v>
+        <v>2.142999887466431</v>
       </c>
       <c r="Q6">
-        <v>1.49399995803833</v>
+        <v>2.164999961853027</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -2326,52 +2326,52 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>1.279000043869019</v>
+        <v>0.6620000004768372</v>
       </c>
       <c r="C7">
-        <v>1.195000052452087</v>
+        <v>0.5210000276565552</v>
       </c>
       <c r="D7">
-        <v>1.371999979019165</v>
+        <v>1.46399998664856</v>
       </c>
       <c r="E7">
-        <v>0.5720000267028809</v>
+        <v>2.924999952316284</v>
       </c>
       <c r="F7">
-        <v>0.1190000027418137</v>
+        <v>2.493000030517578</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>1.062000036239624</v>
+        <v>4.635000228881836</v>
       </c>
       <c r="I7">
-        <v>1.233999967575073</v>
+        <v>1.478999972343445</v>
       </c>
       <c r="J7">
-        <v>1.549000024795532</v>
+        <v>0.3120000064373016</v>
       </c>
       <c r="K7">
-        <v>1.539999961853027</v>
+        <v>0.4329999983310699</v>
       </c>
       <c r="L7">
-        <v>1.271000027656555</v>
+        <v>4.796999931335449</v>
       </c>
       <c r="M7">
-        <v>1.577999949455261</v>
+        <v>2.75600004196167</v>
       </c>
       <c r="N7">
-        <v>0.2630000114440918</v>
+        <v>1.611999988555908</v>
       </c>
       <c r="O7">
-        <v>1.534000039100647</v>
+        <v>1.419000029563904</v>
       </c>
       <c r="P7">
-        <v>1.544999957084656</v>
+        <v>0.800000011920929</v>
       </c>
       <c r="Q7">
-        <v>1.41700005531311</v>
+        <v>0.6079999804496765</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -2379,52 +2379,52 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.3989999890327454</v>
+        <v>5.019999980926514</v>
       </c>
       <c r="C8">
-        <v>0.4589999914169312</v>
+        <v>5.109000205993652</v>
       </c>
       <c r="D8">
-        <v>2.279000043869019</v>
+        <v>3.219000101089478</v>
       </c>
       <c r="E8">
-        <v>1.22599995136261</v>
+        <v>1.896000027656555</v>
       </c>
       <c r="F8">
-        <v>1.13699996471405</v>
+        <v>2.355999946594238</v>
       </c>
       <c r="G8">
-        <v>1.062000036239624</v>
+        <v>4.635000228881836</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>2.184999942779541</v>
+        <v>3.49399995803833</v>
       </c>
       <c r="J8">
-        <v>2.293999910354614</v>
+        <v>4.834000110626221</v>
       </c>
       <c r="K8">
-        <v>0.5070000290870667</v>
+        <v>4.388000011444092</v>
       </c>
       <c r="L8">
-        <v>0.2790000140666962</v>
+        <v>0.2329999953508377</v>
       </c>
       <c r="M8">
-        <v>2.315000057220459</v>
+        <v>2.009000062942505</v>
       </c>
       <c r="N8">
-        <v>0.9900000095367432</v>
+        <v>3.32699990272522</v>
       </c>
       <c r="O8">
-        <v>2.404999971389771</v>
+        <v>3.394999980926514</v>
       </c>
       <c r="P8">
-        <v>0.5289999842643738</v>
+        <v>4.434999942779541</v>
       </c>
       <c r="Q8">
-        <v>0.3580000102519989</v>
+        <v>4.441999912261963</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -2432,52 +2432,52 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>2.263000011444092</v>
+        <v>2.099999904632568</v>
       </c>
       <c r="C9">
-        <v>2.41100001335144</v>
+        <v>1.97599995136261</v>
       </c>
       <c r="D9">
-        <v>0.193000003695488</v>
+        <v>0.5509999990463257</v>
       </c>
       <c r="E9">
-        <v>0.9919999837875366</v>
+        <v>1.644000053405762</v>
       </c>
       <c r="F9">
-        <v>1.230000019073486</v>
+        <v>1.162999987602234</v>
       </c>
       <c r="G9">
-        <v>1.233999967575073</v>
+        <v>1.478999972343445</v>
       </c>
       <c r="H9">
-        <v>2.184999942779541</v>
+        <v>3.49399995803833</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>0.6320000290870667</v>
+        <v>1.666000008583069</v>
       </c>
       <c r="K9">
-        <v>2.690999984741211</v>
+        <v>1.503999948501587</v>
       </c>
       <c r="L9">
-        <v>2.437000036239624</v>
+        <v>3.690000057220459</v>
       </c>
       <c r="M9">
-        <v>0.6579999923706055</v>
+        <v>1.498999953269958</v>
       </c>
       <c r="N9">
-        <v>1.202000021934509</v>
+        <v>0.1809999942779541</v>
       </c>
       <c r="O9">
-        <v>0.3759999871253967</v>
+        <v>0.2509999871253967</v>
       </c>
       <c r="P9">
-        <v>2.568000078201294</v>
+        <v>1.062000036239624</v>
       </c>
       <c r="Q9">
-        <v>2.515000104904175</v>
+        <v>1.039000034332275</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -2485,52 +2485,52 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>2.260999917984009</v>
+        <v>0.6209999918937683</v>
       </c>
       <c r="C10">
-        <v>2.614000082015991</v>
+        <v>0.3400000035762787</v>
       </c>
       <c r="D10">
-        <v>0.492000013589859</v>
+        <v>1.682000041007996</v>
       </c>
       <c r="E10">
-        <v>1.08899998664856</v>
+        <v>3.141999959945679</v>
       </c>
       <c r="F10">
-        <v>1.590000033378601</v>
+        <v>2.700999975204468</v>
       </c>
       <c r="G10">
-        <v>1.549000024795532</v>
+        <v>0.3120000064373016</v>
       </c>
       <c r="H10">
-        <v>2.293999910354614</v>
+        <v>4.834000110626221</v>
       </c>
       <c r="I10">
-        <v>0.6320000290870667</v>
+        <v>1.666000008583069</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <v>2.789999961853027</v>
+        <v>0.5699999928474426</v>
       </c>
       <c r="L10">
-        <v>2.568000078201294</v>
+        <v>4.995999813079834</v>
       </c>
       <c r="M10">
-        <v>0.03700000047683716</v>
+        <v>2.967999935150146</v>
       </c>
       <c r="N10">
-        <v>1.412999987602234</v>
+        <v>1.794000029563904</v>
       </c>
       <c r="O10">
-        <v>0.3600000143051147</v>
+        <v>1.63100004196167</v>
       </c>
       <c r="P10">
-        <v>2.569000005722046</v>
+        <v>1.021999955177307</v>
       </c>
       <c r="Q10">
-        <v>2.57699990272522</v>
+        <v>0.765999972820282</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -2538,52 +2538,52 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.6290000081062317</v>
+        <v>0.6650000214576721</v>
       </c>
       <c r="C11">
-        <v>0.5</v>
+        <v>0.7459999918937683</v>
       </c>
       <c r="D11">
-        <v>2.78600001335144</v>
+        <v>1.340000033378601</v>
       </c>
       <c r="E11">
-        <v>1.730999946594238</v>
+        <v>2.775000095367432</v>
       </c>
       <c r="F11">
-        <v>1.603999972343445</v>
+        <v>2.374000072479248</v>
       </c>
       <c r="G11">
-        <v>1.539999961853027</v>
+        <v>0.4329999983310699</v>
       </c>
       <c r="H11">
-        <v>0.5070000290870667</v>
+        <v>4.388000011444092</v>
       </c>
       <c r="I11">
-        <v>2.690999984741211</v>
+        <v>1.503999948501587</v>
       </c>
       <c r="J11">
-        <v>2.789999961853027</v>
+        <v>0.5699999928474426</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
-        <v>0.2739999890327454</v>
+        <v>4.538000106811523</v>
       </c>
       <c r="M11">
-        <v>2.811000108718872</v>
+        <v>2.598000049591064</v>
       </c>
       <c r="N11">
-        <v>1.493000030517578</v>
+        <v>1.598999977111816</v>
       </c>
       <c r="O11">
-        <v>2.910000085830688</v>
+        <v>1.388000011444092</v>
       </c>
       <c r="P11">
-        <v>0.4560000002384186</v>
+        <v>1.095000028610229</v>
       </c>
       <c r="Q11">
-        <v>0.2549999952316284</v>
+        <v>0.9029999971389771</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -2591,52 +2591,52 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.5600000023841858</v>
+        <v>5.162000179290771</v>
       </c>
       <c r="C12">
-        <v>0.2980000078678131</v>
+        <v>5.264999866485596</v>
       </c>
       <c r="D12">
-        <v>2.538000106811523</v>
+        <v>3.395999908447266</v>
       </c>
       <c r="E12">
-        <v>1.493000030517578</v>
+        <v>2.098000049591064</v>
       </c>
       <c r="F12">
-        <v>1.332000017166138</v>
+        <v>2.558000087738037</v>
       </c>
       <c r="G12">
-        <v>1.271000027656555</v>
+        <v>4.796999931335449</v>
       </c>
       <c r="H12">
-        <v>0.2790000140666962</v>
+        <v>0.2329999953508377</v>
       </c>
       <c r="I12">
-        <v>2.437000036239624</v>
+        <v>3.690000057220459</v>
       </c>
       <c r="J12">
-        <v>2.568000078201294</v>
+        <v>4.995999813079834</v>
       </c>
       <c r="K12">
-        <v>0.2739999890327454</v>
+        <v>4.538000106811523</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>2.589999914169312</v>
+        <v>2.207000017166138</v>
       </c>
       <c r="N12">
-        <v>1.235999941825867</v>
+        <v>3.523000001907349</v>
       </c>
       <c r="O12">
-        <v>2.670000076293945</v>
+        <v>3.582000017166138</v>
       </c>
       <c r="P12">
-        <v>0.5320000052452087</v>
+        <v>4.614999771118164</v>
       </c>
       <c r="Q12">
-        <v>0.2849999964237213</v>
+        <v>4.622000217437744</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -2644,52 +2644,52 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>2.278000116348267</v>
+        <v>3.246000051498413</v>
       </c>
       <c r="C13">
-        <v>2.638000011444092</v>
+        <v>3.259999990463257</v>
       </c>
       <c r="D13">
-        <v>0.5130000114440918</v>
+        <v>1.292999982833862</v>
       </c>
       <c r="E13">
-        <v>1.11300003528595</v>
+        <v>0.1899999976158142</v>
       </c>
       <c r="F13">
-        <v>1.61899995803833</v>
+        <v>0.3589999973773956</v>
       </c>
       <c r="G13">
-        <v>1.577999949455261</v>
+        <v>2.75600004196167</v>
       </c>
       <c r="H13">
-        <v>2.315000057220459</v>
+        <v>2.009000062942505</v>
       </c>
       <c r="I13">
-        <v>0.6579999923706055</v>
+        <v>1.498999953269958</v>
       </c>
       <c r="J13">
-        <v>0.03700000047683716</v>
+        <v>2.967999935150146</v>
       </c>
       <c r="K13">
-        <v>2.811000108718872</v>
+        <v>2.598000049591064</v>
       </c>
       <c r="L13">
-        <v>2.589999914169312</v>
+        <v>2.207000017166138</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
       <c r="N13">
-        <v>1.439000010490417</v>
+        <v>1.33899998664856</v>
       </c>
       <c r="O13">
-        <v>0.3770000040531158</v>
+        <v>1.411999940872192</v>
       </c>
       <c r="P13">
-        <v>2.585000038146973</v>
+        <v>2.453000068664551</v>
       </c>
       <c r="Q13">
-        <v>2.595999956130981</v>
+        <v>2.473999977111816</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -2697,52 +2697,52 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>1.134999990463257</v>
+        <v>2.216000080108643</v>
       </c>
       <c r="C14">
-        <v>1.222000002861023</v>
+        <v>2.108999967575073</v>
       </c>
       <c r="D14">
-        <v>1.312000036239624</v>
+        <v>0.5059999823570251</v>
       </c>
       <c r="E14">
-        <v>0.3519999980926514</v>
+        <v>1.48800003528595</v>
       </c>
       <c r="F14">
-        <v>0.3729999959468842</v>
+        <v>1.004999995231628</v>
       </c>
       <c r="G14">
-        <v>0.2630000114440918</v>
+        <v>1.611999988555908</v>
       </c>
       <c r="H14">
-        <v>0.9900000095367432</v>
+        <v>3.32699990272522</v>
       </c>
       <c r="I14">
-        <v>1.202000021934509</v>
+        <v>0.1809999942779541</v>
       </c>
       <c r="J14">
-        <v>1.412999987602234</v>
+        <v>1.794000029563904</v>
       </c>
       <c r="K14">
-        <v>1.493000030517578</v>
+        <v>1.598999977111816</v>
       </c>
       <c r="L14">
-        <v>1.235999941825867</v>
+        <v>3.523000001907349</v>
       </c>
       <c r="M14">
-        <v>1.439000010490417</v>
+        <v>1.33899998664856</v>
       </c>
       <c r="N14">
         <v>0</v>
       </c>
       <c r="O14">
-        <v>1.455000042915344</v>
+        <v>0.2779999971389771</v>
       </c>
       <c r="P14">
-        <v>1.422000050544739</v>
+        <v>1.236999988555908</v>
       </c>
       <c r="Q14">
-        <v>1.332000017166138</v>
+        <v>1.200999975204468</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -2750,52 +2750,52 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>2.427999973297119</v>
+        <v>2.005000114440918</v>
       </c>
       <c r="C15">
-        <v>2.676000118255615</v>
+        <v>1.929999947547913</v>
       </c>
       <c r="D15">
-        <v>0.2169999927282333</v>
+        <v>0.3140000104904175</v>
       </c>
       <c r="E15">
-        <v>1.179999947547913</v>
+        <v>1.567000031471252</v>
       </c>
       <c r="F15">
-        <v>1.547999978065491</v>
+        <v>1.103999972343445</v>
       </c>
       <c r="G15">
-        <v>1.534000039100647</v>
+        <v>1.419000029563904</v>
       </c>
       <c r="H15">
-        <v>2.404999971389771</v>
+        <v>3.394999980926514</v>
       </c>
       <c r="I15">
-        <v>0.3759999871253967</v>
+        <v>0.2509999871253967</v>
       </c>
       <c r="J15">
-        <v>0.3600000143051147</v>
+        <v>1.63100004196167</v>
       </c>
       <c r="K15">
-        <v>2.910000085830688</v>
+        <v>1.388000011444092</v>
       </c>
       <c r="L15">
-        <v>2.670000076293945</v>
+        <v>3.582000017166138</v>
       </c>
       <c r="M15">
-        <v>0.3770000040531158</v>
+        <v>1.411999940872192</v>
       </c>
       <c r="N15">
-        <v>1.455000042915344</v>
+        <v>0.2779999971389771</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15">
-        <v>2.736999988555908</v>
+        <v>1.074000000953674</v>
       </c>
       <c r="Q15">
-        <v>2.714999914169312</v>
+        <v>1.062999963760376</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -2803,52 +2803,52 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.3210000097751617</v>
+        <v>1.411999940872192</v>
       </c>
       <c r="C16">
-        <v>0.828000009059906</v>
+        <v>1.223999977111816</v>
       </c>
       <c r="D16">
-        <v>2.634999990463257</v>
+        <v>1.258999943733215</v>
       </c>
       <c r="E16">
-        <v>1.577999949455261</v>
+        <v>2.592999935150146</v>
       </c>
       <c r="F16">
-        <v>1.631999969482422</v>
+        <v>2.142999887466431</v>
       </c>
       <c r="G16">
-        <v>1.544999957084656</v>
+        <v>0.800000011920929</v>
       </c>
       <c r="H16">
-        <v>0.5289999842643738</v>
+        <v>4.434999942779541</v>
       </c>
       <c r="I16">
-        <v>2.568000078201294</v>
+        <v>1.062000036239624</v>
       </c>
       <c r="J16">
-        <v>2.569000005722046</v>
+        <v>1.021999955177307</v>
       </c>
       <c r="K16">
-        <v>0.4560000002384186</v>
+        <v>1.095000028610229</v>
       </c>
       <c r="L16">
-        <v>0.5320000052452087</v>
+        <v>4.614999771118164</v>
       </c>
       <c r="M16">
-        <v>2.585000038146973</v>
+        <v>2.453000068664551</v>
       </c>
       <c r="N16">
-        <v>1.422000050544739</v>
+        <v>1.236999988555908</v>
       </c>
       <c r="O16">
-        <v>2.736999988555908</v>
+        <v>1.074000000953674</v>
       </c>
       <c r="P16">
         <v>0</v>
       </c>
       <c r="Q16">
-        <v>0.2509999871253967</v>
+        <v>0.3630000054836273</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -2856,49 +2856,49 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.3770000040531158</v>
+        <v>1.264999985694885</v>
       </c>
       <c r="C17">
-        <v>0.5820000171661377</v>
+        <v>1.032999992370605</v>
       </c>
       <c r="D17">
-        <v>2.599999904632568</v>
+        <v>1.228999972343445</v>
       </c>
       <c r="E17">
-        <v>1.537999987602234</v>
+        <v>2.630000114440918</v>
       </c>
       <c r="F17">
-        <v>1.49399995803833</v>
+        <v>2.164999961853027</v>
       </c>
       <c r="G17">
-        <v>1.41700005531311</v>
+        <v>0.6079999804496765</v>
       </c>
       <c r="H17">
-        <v>0.3580000102519989</v>
+        <v>4.441999912261963</v>
       </c>
       <c r="I17">
-        <v>2.515000104904175</v>
+        <v>1.039000034332275</v>
       </c>
       <c r="J17">
-        <v>2.57699990272522</v>
+        <v>0.765999972820282</v>
       </c>
       <c r="K17">
-        <v>0.2549999952316284</v>
+        <v>0.9029999971389771</v>
       </c>
       <c r="L17">
-        <v>0.2849999964237213</v>
+        <v>4.622000217437744</v>
       </c>
       <c r="M17">
-        <v>2.595999956130981</v>
+        <v>2.473999977111816</v>
       </c>
       <c r="N17">
-        <v>1.332000017166138</v>
+        <v>1.200999975204468</v>
       </c>
       <c r="O17">
-        <v>2.714999914169312</v>
+        <v>1.062999963760376</v>
       </c>
       <c r="P17">
-        <v>0.2509999871253967</v>
+        <v>0.3630000054836273</v>
       </c>
       <c r="Q17">
         <v>0</v>

</xml_diff>